<commit_message>
added some papers and wrote mode into the excel
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topco\Dokumenti\MSc Banking and Digital Finance UCL\Modules\Dissertation\MSc_dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B196B24-8410-4607-A9A7-D13D3E593D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0896F174-7776-4CDB-B8B7-47E1D8C7676B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
   <si>
     <t>Experiment ideas:</t>
   </si>
@@ -202,6 +202,132 @@
   </si>
   <si>
     <t>benchmark data</t>
+  </si>
+  <si>
+    <t>stock prices</t>
+  </si>
+  <si>
+    <t>volatility</t>
+  </si>
+  <si>
+    <t>inflation</t>
+  </si>
+  <si>
+    <t>unemployment</t>
+  </si>
+  <si>
+    <t>gdp</t>
+  </si>
+  <si>
+    <t>interest rates</t>
+  </si>
+  <si>
+    <t>different benchmark models</t>
+  </si>
+  <si>
+    <t>Different data frequencies</t>
+  </si>
+  <si>
+    <t>minute</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>week</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>stable</t>
+  </si>
+  <si>
+    <t>recession</t>
+  </si>
+  <si>
+    <t>Different economic conditions</t>
+  </si>
+  <si>
+    <t>different configuration of the models</t>
+  </si>
+  <si>
+    <t>1045 time series</t>
+  </si>
+  <si>
+    <t>length between 80 and 126</t>
+  </si>
+  <si>
+    <t>from every time-series 18 points were held out</t>
+  </si>
+  <si>
+    <t>one-step-ahead forecasting</t>
+  </si>
+  <si>
+    <t>time-series with different features:</t>
+  </si>
+  <si>
+    <t>seasonality vs non seasonality</t>
+  </si>
+  <si>
+    <t>trend (linear or exponential or none)</t>
+  </si>
+  <si>
+    <t>data pre-processing:</t>
+  </si>
+  <si>
+    <t>log transformation</t>
+  </si>
+  <si>
+    <t>deseasonalization</t>
+  </si>
+  <si>
+    <t>scaling</t>
+  </si>
+  <si>
+    <t>autocorrelation with lag 12 months, using Bartlett formula for confidence</t>
+  </si>
+  <si>
+    <t>results</t>
+  </si>
+  <si>
+    <t>comments on the results</t>
+  </si>
+  <si>
+    <t>average rank</t>
+  </si>
+  <si>
+    <t>SMAPE-TOT (symmetric mean absolute percentage error)</t>
+  </si>
+  <si>
+    <t>FRAC-BEST (fraction-best) - fraction of time series for which a specific model beats all other models</t>
+  </si>
+  <si>
+    <t>SMAPE is used for computing this measure</t>
+  </si>
+  <si>
+    <t>metrics</t>
+  </si>
+  <si>
+    <t>experiment</t>
+  </si>
+  <si>
+    <t>different preprocessing methods</t>
+  </si>
+  <si>
+    <t>data from different domains</t>
+  </si>
+  <si>
+    <t>data with different properties</t>
+  </si>
+  <si>
+    <t>trend, no trend, seasonality, etc…</t>
   </si>
 </sst>
 </file>
@@ -519,22 +645,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:B4"/>
+  <dimension ref="B2:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -544,10 +760,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CAD154-EAE2-4B91-94B1-08EF2FD385B6}">
-  <dimension ref="C4:S41"/>
+  <dimension ref="C4:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -669,6 +885,9 @@
       <c r="K15" t="s">
         <v>26</v>
       </c>
+      <c r="S15" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="16" spans="3:19" x14ac:dyDescent="0.35">
       <c r="D16" t="s">
@@ -677,112 +896,195 @@
       <c r="L16" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="S16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="3:21" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>14</v>
       </c>
       <c r="L17" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="S17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="3:21" x14ac:dyDescent="0.35">
       <c r="D18" t="s">
         <v>13</v>
       </c>
       <c r="L18" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="S18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="3:21" x14ac:dyDescent="0.35">
       <c r="D19" t="s">
         <v>15</v>
       </c>
       <c r="L19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="S19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="3:21" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>16</v>
       </c>
       <c r="K20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="T20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="3:21" x14ac:dyDescent="0.35">
       <c r="L21" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="T21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" x14ac:dyDescent="0.35">
       <c r="L22" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="S22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="3:21" x14ac:dyDescent="0.35">
       <c r="K23" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="T23" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.35">
       <c r="L24" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="T24" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="3:21" x14ac:dyDescent="0.35">
       <c r="L25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="U25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.35">
       <c r="K26" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="27" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="T26" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="3:21" x14ac:dyDescent="0.35">
       <c r="K27" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="28" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="R27" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="28" spans="3:21" x14ac:dyDescent="0.35">
       <c r="K28" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="S28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="T29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="T30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="T31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="3:21" x14ac:dyDescent="0.35">
+      <c r="U32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="S33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="4:21" x14ac:dyDescent="0.35">
       <c r="D34" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="T34" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="T35" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="4:21" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="T36" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="4:21" x14ac:dyDescent="0.35">
       <c r="D37" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="U37" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="4:21" x14ac:dyDescent="0.35">
       <c r="D38" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:21" x14ac:dyDescent="0.35">
       <c r="D39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:21" x14ac:dyDescent="0.35">
       <c r="D40" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:21" x14ac:dyDescent="0.35">
       <c r="D41" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="4:21" x14ac:dyDescent="0.35">
+      <c r="R42" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a few papers and the structure word document
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topco\Dokumenti\MSc Banking and Digital Finance UCL\Modules\Dissertation\MSc_dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0896F174-7776-4CDB-B8B7-47E1D8C7676B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E826B8-1003-4529-BC2F-DA2BA579363D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment Ideas" sheetId="1" r:id="rId1"/>
@@ -763,7 +763,7 @@
   <dimension ref="C4:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+      <selection activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated timeline in excel
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topco\Dokumenti\MSc Banking and Digital Finance UCL\Modules\Dissertation\MSc_dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E826B8-1003-4529-BC2F-DA2BA579363D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112C505C-62FC-4167-98B5-9DB3F2B4B38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12530" yWindow="3820" windowWidth="18670" windowHeight="13070" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment Ideas" sheetId="1" r:id="rId1"/>
     <sheet name="Dissertation Structure" sheetId="2" r:id="rId2"/>
+    <sheet name="Timeline" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
   <si>
     <t>Experiment ideas:</t>
   </si>
@@ -328,16 +329,103 @@
   </si>
   <si>
     <t>trend, no trend, seasonality, etc…</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
+  </si>
+  <si>
+    <t>Week 8</t>
+  </si>
+  <si>
+    <t>Week 9</t>
+  </si>
+  <si>
+    <t>Week 10</t>
+  </si>
+  <si>
+    <t>Week 11</t>
+  </si>
+  <si>
+    <t>Week 12</t>
+  </si>
+  <si>
+    <t>Week 13</t>
+  </si>
+  <si>
+    <t>Week 14</t>
+  </si>
+  <si>
+    <t>Week 15</t>
+  </si>
+  <si>
+    <t>Week 16</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>17-23.6</t>
+  </si>
+  <si>
+    <t>24-30.6</t>
+  </si>
+  <si>
+    <t>1-7.7</t>
+  </si>
+  <si>
+    <t>Finish modularizing all the models</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Think about the different kinds of data, gather them and organize</t>
+  </si>
+  <si>
+    <t>Run models on all data and record all results</t>
+  </si>
+  <si>
+    <t>15-21.7</t>
+  </si>
+  <si>
+    <t>8-14.7</t>
+  </si>
+  <si>
+    <t>Think about fine-tuning the models and hyperparameter selection</t>
+  </si>
+  <si>
+    <t>22-28.7</t>
+  </si>
+  <si>
+    <t>(potentially) create functionality to fine-tune the models</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -762,7 +850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CAD154-EAE2-4B91-94B1-08EF2FD385B6}">
   <dimension ref="C4:U42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
@@ -1090,4 +1178,133 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15A260B7-41A0-4E40-AD6D-CBBD1EEFE9CA}">
+  <dimension ref="C4:F19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F5" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C7" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>119</v>
+      </c>
+      <c r="F8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C14" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed lag llama module and started the presentation
</commit_message>
<xml_diff>
--- a/Experiments.xlsx
+++ b/Experiments.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topco\Dokumenti\MSc Banking and Digital Finance UCL\Modules\Dissertation\MSc_dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{112C505C-62FC-4167-98B5-9DB3F2B4B38C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10D4A6B5-CA34-4880-84F5-39E138C007BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12530" yWindow="3820" windowWidth="18670" windowHeight="13070" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment Ideas" sheetId="1" r:id="rId1"/>
     <sheet name="Dissertation Structure" sheetId="2" r:id="rId2"/>
     <sheet name="Timeline" sheetId="3" r:id="rId3"/>
+    <sheet name="Results structure" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="130">
   <si>
     <t>Experiment ideas:</t>
   </si>
@@ -391,25 +392,43 @@
     <t>Week 2</t>
   </si>
   <si>
-    <t>Think about the different kinds of data, gather them and organize</t>
-  </si>
-  <si>
-    <t>Run models on all data and record all results</t>
-  </si>
-  <si>
     <t>15-21.7</t>
   </si>
   <si>
     <t>8-14.7</t>
   </si>
   <si>
-    <t>Think about fine-tuning the models and hyperparameter selection</t>
-  </si>
-  <si>
     <t>22-28.7</t>
   </si>
   <si>
     <t>(potentially) create functionality to fine-tune the models</t>
+  </si>
+  <si>
+    <t>exchange rates</t>
+  </si>
+  <si>
+    <t>commodity prices</t>
+  </si>
+  <si>
+    <t>crypto prices</t>
+  </si>
+  <si>
+    <t>trading volume</t>
+  </si>
+  <si>
+    <t>real estate prices</t>
+  </si>
+  <si>
+    <t>market sentiment data?</t>
+  </si>
+  <si>
+    <t>Time series cross validation</t>
+  </si>
+  <si>
+    <t>Complete the draft presentation, add table comparison to the notebook, add history to the predictions plot</t>
+  </si>
+  <si>
+    <t>lag-llama fine tune and timeGPT</t>
   </si>
 </sst>
 </file>
@@ -733,111 +752,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:C26"/>
+  <dimension ref="B2:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C17" t="s">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C18" t="s">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C19" t="s">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C20" t="s">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C21" t="s">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C22" t="s">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C25" t="s">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
-      <c r="C26" t="s">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>69</v>
       </c>
     </row>
@@ -854,9 +903,9 @@
       <selection activeCell="V38" sqref="V38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>2</v>
       </c>
@@ -867,7 +916,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -878,7 +927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="7" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -889,7 +938,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="8" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>4</v>
       </c>
@@ -900,7 +949,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="9" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>5</v>
       </c>
@@ -911,7 +960,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="10" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>7</v>
       </c>
@@ -922,7 +971,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>8</v>
       </c>
@@ -933,7 +982,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>9</v>
       </c>
@@ -944,7 +993,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>9</v>
       </c>
@@ -955,7 +1004,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>10</v>
       </c>
@@ -966,7 +1015,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>11</v>
       </c>
@@ -977,7 +1026,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="3:19" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:19" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>12</v>
       </c>
@@ -988,7 +1037,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>14</v>
       </c>
@@ -999,7 +1048,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
         <v>13</v>
       </c>
@@ -1010,7 +1059,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>15</v>
       </c>
@@ -1021,7 +1070,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:21" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>16</v>
       </c>
@@ -1032,7 +1081,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:21" x14ac:dyDescent="0.25">
       <c r="L21" t="s">
         <v>32</v>
       </c>
@@ -1040,7 +1089,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:21" x14ac:dyDescent="0.25">
       <c r="L22" t="s">
         <v>33</v>
       </c>
@@ -1048,7 +1097,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="23" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:21" x14ac:dyDescent="0.25">
       <c r="K23" t="s">
         <v>34</v>
       </c>
@@ -1056,7 +1105,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:21" x14ac:dyDescent="0.25">
       <c r="L24" t="s">
         <v>35</v>
       </c>
@@ -1064,7 +1113,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:21" x14ac:dyDescent="0.25">
       <c r="L25" t="s">
         <v>36</v>
       </c>
@@ -1072,7 +1121,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:21" x14ac:dyDescent="0.25">
       <c r="K26" t="s">
         <v>37</v>
       </c>
@@ -1080,7 +1129,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="27" spans="3:21" x14ac:dyDescent="0.25">
       <c r="K27" t="s">
         <v>38</v>
       </c>
@@ -1088,7 +1137,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="28" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="28" spans="3:21" x14ac:dyDescent="0.25">
       <c r="K28" t="s">
         <v>39</v>
       </c>
@@ -1096,32 +1145,32 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:21" x14ac:dyDescent="0.25">
       <c r="T29" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:21" x14ac:dyDescent="0.25">
       <c r="T30" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:21" x14ac:dyDescent="0.25">
       <c r="T31" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="3:21" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:21" x14ac:dyDescent="0.25">
       <c r="U32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="4:21" x14ac:dyDescent="0.35">
+    <row r="33" spans="4:21" x14ac:dyDescent="0.25">
       <c r="S33" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="4:21" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>40</v>
       </c>
@@ -1129,12 +1178,12 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="4:21" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:21" x14ac:dyDescent="0.25">
       <c r="T35" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="4:21" x14ac:dyDescent="0.35">
+    <row r="36" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>3</v>
       </c>
@@ -1142,7 +1191,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="37" spans="4:21" x14ac:dyDescent="0.35">
+    <row r="37" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>41</v>
       </c>
@@ -1150,27 +1199,27 @@
         <v>96</v>
       </c>
     </row>
-    <row r="38" spans="4:21" x14ac:dyDescent="0.35">
+    <row r="38" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D38" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="39" spans="4:21" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="40" spans="4:21" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="4:21" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="42" spans="4:21" x14ac:dyDescent="0.35">
+    <row r="42" spans="4:21" x14ac:dyDescent="0.25">
       <c r="R42" t="s">
         <v>86</v>
       </c>
@@ -1185,12 +1234,12 @@
   <dimension ref="C4:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>111</v>
       </c>
@@ -1198,7 +1247,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>116</v>
       </c>
@@ -1209,7 +1258,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>97</v>
       </c>
@@ -1217,88 +1266,88 @@
         <v>114</v>
       </c>
       <c r="F6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.35">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>100</v>
       </c>
       <c r="D9" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>110</v>
       </c>
@@ -1307,4 +1356,18 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDA7D52E-B1CC-4EE6-9FE8-0A7B1DC12AF2}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>